<commit_message>
Add StepMotor Music Player Function
</commit_message>
<xml_diff>
--- a/Protocol_NeodAnderjon_20180629pm1847.xlsx
+++ b/Protocol_NeodAnderjon_20180629pm1847.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2490DA9-E0D1-4ED4-94FA-15361B214EEE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E39011-2432-41E3-A952-BE0538CE4A41}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>AA</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -489,6 +489,559 @@
   </si>
   <si>
     <r>
+      <t>EmbeddedBreakerCore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>原生</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>皇后数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>配置编号</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MotorMotionController</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运动算例调用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>API</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>动作</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>行距</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>速度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>最大</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>9999</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第一组倍数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第二组倍数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第三组倍数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第四组倍数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>第五组倍数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>位</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Ubuntu Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音乐模式有限无限</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音频放大系数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>节拍放大系数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">04 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>音乐</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">00 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有限</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">01 </t>
     </r>
     <r>
@@ -499,278 +1052,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>正转</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">02 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>反转</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>EmbeddedBreakerCore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>原生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>API</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>皇后数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>配置编号</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>MotorMotionController</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>运动算例调用</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>API</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>动作</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>行距</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>速度</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
+      <t>无限</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -792,212 +1074,7 @@
         <rFont val="Ubuntu Mono"/>
         <family val="3"/>
       </rPr>
-      <t>9999</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第一组倍数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第二组倍数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第三组倍数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第四组倍数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>第五组倍数</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>(2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>位</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
+      <t>09</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1397,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1418,16 +1495,16 @@
     <col min="11" max="11" width="8.88671875" style="1"/>
     <col min="12" max="12" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="1"/>
+    <col min="17" max="17" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
@@ -1479,7 +1556,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>3</v>
@@ -1493,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>3</v>
@@ -1520,7 +1597,7 @@
     </row>
     <row r="10" spans="1:18" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
@@ -1531,19 +1608,28 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>8</v>
@@ -1563,13 +1649,22 @@
         <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>1</v>
@@ -1585,6 +1680,9 @@
       <c r="N13" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="O13" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
@@ -1597,78 +1695,83 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="L17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="O17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R16" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="3:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>